<commit_message>
Telecom, Geofísica, Biomédicos, industrial
</commit_message>
<xml_diff>
--- a/CLAVES GEOFÍSICA.xlsx
+++ b/CLAVES GEOFÍSICA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultad\Servicio Social\FORMATOS FINALES CORREGIDOS COMPLETOS\PlanesEstudio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ss\PlanesEstudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GEOFÍSICA!$A$1:$Q$89</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="158">
   <si>
     <t>CLAVE DGAE</t>
   </si>
@@ -485,16 +485,19 @@
     <t>COORDINACIÓN DE CIENCIAS APLICADAS</t>
   </si>
   <si>
-    <t>INGENIERÍA GEOLÓGICA</t>
+    <t>INGENIERÍA  GEOLÓGICA</t>
   </si>
   <si>
     <t>INGENIERÍA EN COMPUTACIÓN</t>
   </si>
   <si>
+    <t>INGENIERÍA  GEOFÍSICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA MECATRÓNICA</t>
+  </si>
+  <si>
     <t>GEODESIA</t>
-  </si>
-  <si>
-    <t>INGENIERÍA MECATRÓNICA</t>
   </si>
   <si>
     <t>INGENIERÍA INDUSTRIAL</t>
@@ -503,7 +506,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -547,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -607,32 +610,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -683,18 +666,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -982,16 +953,18 @@
   </sheetPr>
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T81" sqref="T81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="29" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="28" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="15" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
@@ -1002,7 +975,7 @@
     <col min="15" max="15" width="15.42578125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="42.85546875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="47.140625" customWidth="1"/>
+    <col min="18" max="18" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="22.5" x14ac:dyDescent="0.25">
@@ -1113,7 +1086,7 @@
       <c r="Q2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1169,7 +1142,7 @@
       <c r="Q3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1225,7 +1198,7 @@
       <c r="Q4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1281,7 +1254,7 @@
       <c r="Q5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1337,7 +1310,7 @@
       <c r="Q6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1393,7 +1366,7 @@
       <c r="Q7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="R7" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1450,7 +1423,7 @@
       <c r="Q8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1507,7 +1480,7 @@
       <c r="Q9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="21" t="s">
+      <c r="R9" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1564,7 +1537,7 @@
       <c r="Q10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="21" t="s">
+      <c r="R10" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1621,7 +1594,7 @@
       <c r="Q11" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R11" s="21" t="s">
+      <c r="R11" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1678,7 +1651,7 @@
       <c r="Q12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R12" s="21" t="s">
+      <c r="R12" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1735,7 +1708,7 @@
       <c r="Q13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="21" t="s">
+      <c r="R13" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1792,7 +1765,7 @@
       <c r="Q14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="R14" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1849,7 +1822,7 @@
       <c r="Q15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="21" t="s">
+      <c r="R15" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1906,7 +1879,7 @@
       <c r="Q16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="21" t="s">
+      <c r="R16" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1963,7 +1936,7 @@
       <c r="Q17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="21" t="s">
+      <c r="R17" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2020,7 +1993,7 @@
       <c r="Q18" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R18" s="21" t="s">
+      <c r="R18" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2077,7 +2050,7 @@
       <c r="Q19" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R19" s="21" t="s">
+      <c r="R19" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2134,7 +2107,7 @@
       <c r="Q20" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="R20" s="21" t="s">
+      <c r="R20" s="10" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2191,7 +2164,7 @@
       <c r="Q21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R21" s="21" t="s">
+      <c r="R21" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2248,7 +2221,7 @@
       <c r="Q22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="21" t="s">
+      <c r="R22" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2305,7 +2278,7 @@
       <c r="Q23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R23" s="21" t="s">
+      <c r="R23" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2362,7 +2335,7 @@
       <c r="Q24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R24" s="21" t="s">
+      <c r="R24" s="10" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2419,7 +2392,7 @@
       <c r="Q25" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R25" s="21" t="s">
+      <c r="R25" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2476,8 +2449,8 @@
       <c r="Q26" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R26" s="21" t="s">
-        <v>27</v>
+      <c r="R26" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2533,7 +2506,7 @@
       <c r="Q27" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R27" s="21" t="s">
+      <c r="R27" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2590,7 +2563,7 @@
       <c r="Q28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R28" s="21" t="s">
+      <c r="R28" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2647,8 +2620,8 @@
       <c r="Q29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R29" s="21" t="s">
-        <v>27</v>
+      <c r="R29" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2704,8 +2677,8 @@
       <c r="Q30" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R30" s="21" t="s">
-        <v>27</v>
+      <c r="R30" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2761,8 +2734,8 @@
       <c r="Q31" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R31" s="21" t="s">
-        <v>27</v>
+      <c r="R31" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2818,7 +2791,7 @@
       <c r="Q32" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R32" s="21" t="s">
+      <c r="R32" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2875,8 +2848,8 @@
       <c r="Q33" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R33" s="21" t="s">
-        <v>27</v>
+      <c r="R33" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2932,8 +2905,8 @@
       <c r="Q34" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R34" s="21" t="s">
-        <v>27</v>
+      <c r="R34" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2989,7 +2962,7 @@
       <c r="Q35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R35" s="21" t="s">
+      <c r="R35" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3046,8 +3019,8 @@
       <c r="Q36" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R36" s="21" t="s">
-        <v>27</v>
+      <c r="R36" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3103,7 +3076,7 @@
       <c r="Q37" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R37" s="21" t="s">
+      <c r="R37" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3160,8 +3133,8 @@
       <c r="Q38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R38" s="21" t="s">
-        <v>27</v>
+      <c r="R38" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3217,8 +3190,8 @@
       <c r="Q39" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R39" s="21" t="s">
-        <v>27</v>
+      <c r="R39" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3274,8 +3247,8 @@
       <c r="Q40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R40" s="21" t="s">
-        <v>27</v>
+      <c r="R40" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3331,7 +3304,7 @@
       <c r="Q41" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R41" s="21" t="s">
+      <c r="R41" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3388,8 +3361,8 @@
       <c r="Q42" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R42" s="21" t="s">
-        <v>27</v>
+      <c r="R42" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3445,8 +3418,8 @@
       <c r="Q43" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R43" s="21" t="s">
-        <v>27</v>
+      <c r="R43" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3502,8 +3475,8 @@
       <c r="Q44" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R44" s="21" t="s">
-        <v>27</v>
+      <c r="R44" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3559,7 +3532,7 @@
       <c r="Q45" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R45" s="21" t="s">
+      <c r="R45" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3616,8 +3589,8 @@
       <c r="Q46" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R46" s="21" t="s">
-        <v>27</v>
+      <c r="R46" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3673,8 +3646,8 @@
       <c r="Q47" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R47" s="21" t="s">
-        <v>27</v>
+      <c r="R47" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3730,8 +3703,8 @@
       <c r="Q48" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R48" s="21" t="s">
-        <v>27</v>
+      <c r="R48" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3787,7 +3760,7 @@
       <c r="Q49" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R49" s="21" t="s">
+      <c r="R49" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3844,8 +3817,8 @@
       <c r="Q50" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R50" s="21" t="s">
-        <v>27</v>
+      <c r="R50" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3901,8 +3874,8 @@
       <c r="Q51" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R51" s="21" t="s">
-        <v>27</v>
+      <c r="R51" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3957,7 +3930,7 @@
       <c r="Q52" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R52" s="21" t="s">
+      <c r="R52" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4013,7 +3986,7 @@
       <c r="Q53" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R53" s="21" t="s">
+      <c r="R53" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4069,7 +4042,7 @@
       <c r="Q54" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R54" s="21" t="s">
+      <c r="R54" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4125,7 +4098,7 @@
       <c r="Q55" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R55" s="21" t="s">
+      <c r="R55" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4181,7 +4154,7 @@
       <c r="Q56" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R56" s="21" t="s">
+      <c r="R56" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4237,7 +4210,7 @@
       <c r="Q57" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R57" s="21" t="s">
+      <c r="R57" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4293,7 +4266,7 @@
       <c r="Q58" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R58" s="21" t="s">
+      <c r="R58" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4349,7 +4322,7 @@
       <c r="Q59" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R59" s="21" t="s">
+      <c r="R59" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4405,7 +4378,7 @@
       <c r="Q60" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="R60" s="21" t="s">
+      <c r="R60" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4463,7 +4436,7 @@
       <c r="Q61" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R61" s="21" t="s">
+      <c r="R61" s="10" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4521,7 +4494,7 @@
       <c r="Q62" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="R62" s="22" t="s">
+      <c r="R62" s="10" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4579,7 +4552,7 @@
       <c r="Q63" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="R63" s="22" t="s">
+      <c r="R63" s="10" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4637,8 +4610,8 @@
       <c r="Q64" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="R64" s="22" t="s">
-        <v>154</v>
+      <c r="R64" s="10" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -4695,8 +4668,8 @@
       <c r="Q65" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="R65" s="22" t="s">
-        <v>154</v>
+      <c r="R65" s="10" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -4753,7 +4726,7 @@
       <c r="Q66" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R66" s="23" t="s">
+      <c r="R66" s="10" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4811,8 +4784,8 @@
       <c r="Q67" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R67" s="24" t="s">
-        <v>156</v>
+      <c r="R67" s="10" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4868,7 +4841,7 @@
       <c r="Q68" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R68" s="24" t="s">
+      <c r="R68" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4925,8 +4898,8 @@
       <c r="Q69" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R69" s="24" t="s">
-        <v>27</v>
+      <c r="R69" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4982,8 +4955,8 @@
       <c r="Q70" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R70" s="24" t="s">
-        <v>27</v>
+      <c r="R70" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5039,7 +5012,7 @@
       <c r="Q71" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R71" s="23" t="s">
+      <c r="R71" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5096,7 +5069,7 @@
       <c r="Q72" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R72" s="23" t="s">
+      <c r="R72" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5153,7 +5126,7 @@
       <c r="Q73" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R73" s="23" t="s">
+      <c r="R73" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5210,7 +5183,7 @@
       <c r="Q74" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R74" s="24" t="s">
+      <c r="R74" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5267,7 +5240,7 @@
       <c r="Q75" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R75" s="24" t="s">
+      <c r="R75" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5324,8 +5297,8 @@
       <c r="Q76" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R76" s="23" t="s">
-        <v>27</v>
+      <c r="R76" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5381,7 +5354,7 @@
       <c r="Q77" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R77" s="24" t="s">
+      <c r="R77" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5438,7 +5411,7 @@
       <c r="Q78" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R78" s="23" t="s">
+      <c r="R78" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5495,8 +5468,8 @@
       <c r="Q79" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R79" s="23" t="s">
-        <v>27</v>
+      <c r="R79" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5552,8 +5525,8 @@
       <c r="Q80" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R80" s="23" t="s">
-        <v>27</v>
+      <c r="R80" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5609,8 +5582,8 @@
       <c r="Q81" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R81" s="23" t="s">
-        <v>27</v>
+      <c r="R81" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5666,7 +5639,7 @@
       <c r="Q82" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R82" s="23" t="s">
+      <c r="R82" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5723,8 +5696,8 @@
       <c r="Q83" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R83" s="23" t="s">
-        <v>27</v>
+      <c r="R83" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5780,8 +5753,8 @@
       <c r="Q84" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R84" s="23" t="s">
-        <v>27</v>
+      <c r="R84" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5837,7 +5810,7 @@
       <c r="Q85" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R85" s="23" t="s">
+      <c r="R85" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5894,8 +5867,8 @@
       <c r="Q86" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R86" s="23" t="s">
-        <v>27</v>
+      <c r="R86" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5951,7 +5924,7 @@
       <c r="Q87" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R87" s="24" t="s">
+      <c r="R87" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6008,8 +5981,8 @@
       <c r="Q88" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R88" s="23" t="s">
-        <v>27</v>
+      <c r="R88" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -6065,12 +6038,11 @@
       <c r="Q89" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="R89" s="23" t="s">
+      <c r="R89" s="10" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q89"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="41" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>